<commit_message>
Experiments with Excel sheet -- Print all values
</commit_message>
<xml_diff>
--- a/test/utils/test.xlsx
+++ b/test/utils/test.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
+    <sheet name="SecondTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>test1</t>
   </si>
@@ -78,6 +79,12 @@
   </si>
   <si>
     <t>password6</t>
+  </si>
+  <si>
+    <t>dataSheet</t>
+  </si>
+  <si>
+    <t>firstTable</t>
   </si>
 </sst>
 </file>
@@ -406,7 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
@@ -523,4 +530,27 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>